<commit_message>
fix minor problems air cargo + results for some tests
</commit_message>
<xml_diff>
--- a/P3/Helper.xlsx
+++ b/P3/Helper.xlsx
@@ -4,10 +4,12 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Definitions" sheetId="1" r:id="rId1"/>
+    <sheet name="Results" sheetId="2" r:id="rId2"/>
+    <sheet name="Config" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="33">
   <si>
     <t>SFO</t>
   </si>
@@ -61,6 +63,63 @@
   </si>
   <si>
     <t>C4</t>
+  </si>
+  <si>
+    <t>Problem</t>
+  </si>
+  <si>
+    <t>Problems</t>
+  </si>
+  <si>
+    <t>Algorithms</t>
+  </si>
+  <si>
+    <t>breadth_first_search</t>
+  </si>
+  <si>
+    <t>breadth_first_tree_search</t>
+  </si>
+  <si>
+    <t>depth_first_graph_search</t>
+  </si>
+  <si>
+    <t>depth_limited_search</t>
+  </si>
+  <si>
+    <t>uniform_cost_search</t>
+  </si>
+  <si>
+    <t>Algorithm</t>
+  </si>
+  <si>
+    <t>Expansions</t>
+  </si>
+  <si>
+    <t>Goal Tests</t>
+  </si>
+  <si>
+    <t>New Nodes</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Plan length</t>
+  </si>
+  <si>
+    <t>astar_search - h_1</t>
+  </si>
+  <si>
+    <t>astar_search - h_ignore_preconditions</t>
+  </si>
+  <si>
+    <t>astar_search - h_pg_levelsum</t>
+  </si>
+  <si>
+    <t>greedy_best_first_graph_search - h_1</t>
+  </si>
+  <si>
+    <t>recursive_best_first_search - h_1</t>
   </si>
 </sst>
 </file>
@@ -116,12 +175,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -404,25 +466,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -451,21 +513,21 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C10" s="2" t="s">
+      <c r="B10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>6</v>
       </c>
     </row>
@@ -505,24 +567,24 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
+      <c r="A18" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C19" s="2" t="s">
+      <c r="B19" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D19" s="1" t="s">
         <v>12</v>
       </c>
     </row>
@@ -573,4 +635,554 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="35.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2">
+        <v>43</v>
+      </c>
+      <c r="D2">
+        <v>56</v>
+      </c>
+      <c r="E2">
+        <v>180</v>
+      </c>
+      <c r="F2">
+        <v>6</v>
+      </c>
+      <c r="G2">
+        <v>2.7699999999999999E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3">
+        <v>1458</v>
+      </c>
+      <c r="D3">
+        <v>1459</v>
+      </c>
+      <c r="E3">
+        <v>5960</v>
+      </c>
+      <c r="F3">
+        <v>6</v>
+      </c>
+      <c r="G3">
+        <v>0.81410000000000005</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4">
+        <v>21</v>
+      </c>
+      <c r="D4">
+        <v>22</v>
+      </c>
+      <c r="E4">
+        <v>84</v>
+      </c>
+      <c r="F4">
+        <v>20</v>
+      </c>
+      <c r="G4">
+        <v>1.29E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5">
+        <v>101</v>
+      </c>
+      <c r="D5">
+        <v>271</v>
+      </c>
+      <c r="E5">
+        <v>414</v>
+      </c>
+      <c r="F5">
+        <v>50</v>
+      </c>
+      <c r="G5">
+        <v>8.0399999999999999E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6">
+        <v>55</v>
+      </c>
+      <c r="D6">
+        <v>57</v>
+      </c>
+      <c r="E6">
+        <v>224</v>
+      </c>
+      <c r="F6">
+        <v>6</v>
+      </c>
+      <c r="G6">
+        <v>3.3700000000000001E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7">
+        <v>4229</v>
+      </c>
+      <c r="D7">
+        <v>4230</v>
+      </c>
+      <c r="E7">
+        <v>17023</v>
+      </c>
+      <c r="F7">
+        <v>6</v>
+      </c>
+      <c r="G7">
+        <v>2.4195000000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8">
+        <v>7</v>
+      </c>
+      <c r="D8">
+        <v>9</v>
+      </c>
+      <c r="E8">
+        <v>28</v>
+      </c>
+      <c r="F8">
+        <v>6</v>
+      </c>
+      <c r="G8">
+        <v>4.4999999999999997E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9">
+        <v>55</v>
+      </c>
+      <c r="D9">
+        <v>57</v>
+      </c>
+      <c r="E9">
+        <v>224</v>
+      </c>
+      <c r="F9">
+        <v>6</v>
+      </c>
+      <c r="G9">
+        <v>3.27E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10">
+        <v>41</v>
+      </c>
+      <c r="D10">
+        <v>43</v>
+      </c>
+      <c r="E10">
+        <v>170</v>
+      </c>
+      <c r="F10">
+        <v>6</v>
+      </c>
+      <c r="G10">
+        <v>3.3300000000000003E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>2</v>
+      </c>
+      <c r="B12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12">
+        <v>3346</v>
+      </c>
+      <c r="D12">
+        <v>4612</v>
+      </c>
+      <c r="E12">
+        <v>30534</v>
+      </c>
+      <c r="F12">
+        <v>9</v>
+      </c>
+      <c r="G12">
+        <v>12.180199999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>2</v>
+      </c>
+      <c r="B13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>2</v>
+      </c>
+      <c r="B14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>2</v>
+      </c>
+      <c r="B15" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>2</v>
+      </c>
+      <c r="B16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>2</v>
+      </c>
+      <c r="B17" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>2</v>
+      </c>
+      <c r="B18" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>2</v>
+      </c>
+      <c r="B19" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>2</v>
+      </c>
+      <c r="B20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>2</v>
+      </c>
+      <c r="B21" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>3</v>
+      </c>
+      <c r="B22" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>3</v>
+      </c>
+      <c r="B23" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>3</v>
+      </c>
+      <c r="B24" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>3</v>
+      </c>
+      <c r="B25" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>3</v>
+      </c>
+      <c r="B26" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>3</v>
+      </c>
+      <c r="B27" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>3</v>
+      </c>
+      <c r="B28" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>3</v>
+      </c>
+      <c r="B29" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>3</v>
+      </c>
+      <c r="B30" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>3</v>
+      </c>
+      <c r="B31" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A1:A1048576">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color theme="6" tint="0.79998168889431442"/>
+        <color theme="7" tint="0.79998168889431442"/>
+        <color theme="9" tint="0.79998168889431442"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Config!$A$2:$A$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>A1:A1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Config!$B$2:$B$11</xm:f>
+          </x14:formula1>
+          <xm:sqref>B1:B1048576</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="32.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>